<commit_message>
Migrate to MySQL, fix dashboard year filter, and optimize performance
</commit_message>
<xml_diff>
--- a/backend/missing_cogs_report.xlsx
+++ b/backend/missing_cogs_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,21 +443,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PRCC-40102 HV GOLD T350 CT VN-200KK</t>
+          <t>DW-500 NT 740 DELICIOUS -18LP</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PCL-31300 BLUE OR 50 PASTE VN-4K</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DI-400 019-1 BELIZE BREEZE-18LP</t>
+          <t>PFT-253 QUARTZ GREY RAL 7039 VN-20KSP</t>
         </is>
       </c>
     </row>

</xml_diff>